<commit_message>
[Fix] Jason Data, MonsterManager
</commit_message>
<xml_diff>
--- a/excel2json-master/FieldMonster_Data.xlsx
+++ b/excel2json-master/FieldMonster_Data.xlsx
@@ -1,33 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\이영선\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\unity\TeamProject\05TeamProject14\Project_P\excel2json-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C680ACC-752D-4002-944D-7D9687EBA33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B788962-7EE2-4FA8-A730-FB24D60D9625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{72DB4AE2-8199-4472-B082-34F26D3D5631}"/>
+    <workbookView xWindow="4875" yWindow="1800" windowWidth="21600" windowHeight="11205" xr2:uid="{72DB4AE2-8199-4472-B082-34F26D3D5631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -36,13 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
-    <t>#FieldMonster{{}}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$key</t>
-  </si>
-  <si>
     <t>level</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -106,6 +90,14 @@
   </si>
   <si>
     <t>BullA</t>
+  </si>
+  <si>
+    <t>#FieldMonster[{}]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -505,7 +497,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:C17"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -520,48 +512,48 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -599,7 +591,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -637,7 +629,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -675,7 +667,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -713,7 +705,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
@@ -751,7 +743,7 @@
     </row>
     <row r="7" spans="1:13">
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
@@ -789,7 +781,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1">
         <v>5</v>

</xml_diff>

<commit_message>
[feat] Monster FSM 중간저장_v1
</commit_message>
<xml_diff>
--- a/excel2json-master/FieldMonster_Data.xlsx
+++ b/excel2json-master/FieldMonster_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\unity\TeamProject\05TeamProject14\Project_P\excel2json-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\이영선\Desktop\Sparta_Club\Project_P\Project_P\excel2json-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B788962-7EE2-4FA8-A730-FB24D60D9625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAF14D9-E1E8-4C05-9FCA-C042DB9EABC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4875" yWindow="1800" windowWidth="21600" windowHeight="11205" xr2:uid="{72DB4AE2-8199-4472-B082-34F26D3D5631}"/>
+    <workbookView xWindow="1605" yWindow="2820" windowWidth="23655" windowHeight="9765" xr2:uid="{72DB4AE2-8199-4472-B082-34F26D3D5631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>level</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>exp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>AtkStance</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -59,14 +51,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Speed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AtkSpeed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Range</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -96,7 +80,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>name</t>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MoveSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MonsterID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RunSpeed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -164,7 +168,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -179,6 +183,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,326 +501,352 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4297DAEF-F778-44C4-9BC9-6DB94BE857D0}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="L1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:14">
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>100</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>100</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>150</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>150</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:13">
-      <c r="B2" s="2" t="s">
+    <row r="6" spans="1:14">
+      <c r="B6" s="5">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <v>100</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>225</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>7</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="B7" s="5">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1">
         <v>4</v>
       </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
-        <v>1</v>
-      </c>
-      <c r="L2" s="1">
+      <c r="E7" s="1">
+        <v>450</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>8</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M2" s="1">
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N7" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>100</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>4</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
+    <row r="8" spans="1:14">
+      <c r="B8" s="5">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1">
+        <v>900</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>10</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
-        <v>1</v>
-      </c>
-      <c r="L3" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1">
-        <v>150</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>5</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1">
-        <v>1</v>
-      </c>
-      <c r="L4" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="M4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1">
-        <v>150</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>5</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1.25</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="M5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1">
-        <v>225</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>7</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>1</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1">
-        <v>1</v>
-      </c>
-      <c r="L6" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="M6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1">
-        <v>4</v>
-      </c>
-      <c r="D7" s="1">
-        <v>450</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>8</v>
-      </c>
-      <c r="G7" s="1">
-        <v>2</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1">
-        <v>1</v>
-      </c>
-      <c r="L7" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="M7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="B8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="1">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1">
-        <v>900</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>10</v>
-      </c>
-      <c r="G8" s="1">
-        <v>2.25</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1">
-        <v>1</v>
-      </c>
-      <c r="L8" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="M8" s="1">
+      <c r="N8" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Feat] TargetRange , Damping 추가
</commit_message>
<xml_diff>
--- a/excel2json-master/FieldMonster_Data.xlsx
+++ b/excel2json-master/FieldMonster_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\이영선\Desktop\Sparta_Club\Project_P\Project_P\excel2json-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705C055E-98BF-4C38-91E6-6C97CDA599BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6494E75-D9FE-4DA7-8E9F-E76A4240AB5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{72DB4AE2-8199-4472-B082-34F26D3D5631}"/>
   </bookViews>
@@ -24,8 +24,111 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>이영선</author>
+  </authors>
+  <commentList>
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{4E868B25-EC9E-4419-9CFD-CFC61C7C719D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>플레이어와의</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>거리</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{EF0C0921-123B-4A88-9153-A33F3084D053}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>몬스터</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>어그로</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>범위</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>AtkStance</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,10 +154,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Range</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>#FieldMonster[{}]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -139,6 +238,18 @@
   </si>
   <si>
     <t>Monsters/BullA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtkRange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TargetRange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RotationDamping</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -146,7 +257,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +287,21 @@
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="3">
@@ -538,11 +664,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4297DAEF-F778-44C4-9BC9-6DB94BE857D0}">
-  <dimension ref="A1:O8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4297DAEF-F778-44C4-9BC9-6DB94BE857D0}">
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -555,23 +681,25 @@
     <col min="12" max="12" width="11.625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>0</v>
@@ -592,24 +720,30 @@
         <v>5</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="B2" s="5">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -642,18 +776,24 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="N2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="P2" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:17">
       <c r="B3" s="5">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -686,18 +826,24 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="N3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="P3" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:17">
       <c r="B4" s="5">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
@@ -730,18 +876,24 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="N4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="P4" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:17">
       <c r="B5" s="5">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
@@ -774,18 +926,24 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="N5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="B6" s="5">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="B6" s="5">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="D6" s="1">
         <v>3</v>
@@ -818,18 +976,24 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="N6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="P6" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:17">
       <c r="B7" s="5">
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="1">
         <v>4</v>
@@ -862,18 +1026,24 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="N7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="P7" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:17">
       <c r="B8" s="5">
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1">
         <v>5</v>
@@ -906,14 +1076,21 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="N8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="P8" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Fix] 일반 몬스터 PrefabPath 수정
</commit_message>
<xml_diff>
--- a/excel2json-master/FieldMonster_Data.xlsx
+++ b/excel2json-master/FieldMonster_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\이영선\Desktop\Sparta_Club\Project_P\Project_P\excel2json-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6494E75-D9FE-4DA7-8E9F-E76A4240AB5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2431E795-3137-4221-B7C8-B2B9DCA3D376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{72DB4AE2-8199-4472-B082-34F26D3D5631}"/>
   </bookViews>
@@ -189,58 +189,30 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Monsters/PlatypusA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ChameleonA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Monsters/ChameleonA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Meerkat</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Monsters/Meerkat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Porcupine</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Monsters/Porcupine</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Skunk</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Monsters/Skunk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>WolfA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Monsters/WolfA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BullA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Monsters/BullA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>AtkRange</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -250,6 +222,34 @@
   </si>
   <si>
     <t>RotationDamping</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monsters/PlatypusA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monsters/ChameleonA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monsters/Meerkat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monsters/Porcupine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monsters/Skunk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monsters/WolfA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monsters/BullA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -668,7 +668,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -726,16 +726,16 @@
         <v>12</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>13</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -779,7 +779,7 @@
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="P2" s="1">
         <v>5</v>
@@ -793,7 +793,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -829,7 +829,7 @@
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="P3" s="1">
         <v>5</v>
@@ -843,7 +843,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
@@ -879,7 +879,7 @@
         <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="P4" s="1">
         <v>5</v>
@@ -893,7 +893,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
@@ -929,7 +929,7 @@
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="P5" s="1">
         <v>5</v>
@@ -943,7 +943,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1">
         <v>3</v>
@@ -979,7 +979,7 @@
         <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="P6" s="1">
         <v>5</v>
@@ -993,7 +993,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1">
         <v>4</v>
@@ -1029,7 +1029,7 @@
         <v>1</v>
       </c>
       <c r="O7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="P7" s="1">
         <v>5</v>
@@ -1043,7 +1043,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1">
         <v>5</v>
@@ -1079,7 +1079,7 @@
         <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="P8" s="1">
         <v>5</v>

</xml_diff>